<commit_message>
bcThang - Cập nhật dữ liệu phụ lục
</commit_message>
<xml_diff>
--- a/ToolBaoCao/App_Data/plthang.xlsx
+++ b/ToolBaoCao/App_Data/plthang.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\TaiLieu\240925\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\AChuong\ToolBaoCao\ToolBaoCao\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1484B184-6BCC-4848-8C8A-FF251A9F40CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB95FCAA-82E7-437E-9111-74EC45E30550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12375" yWindow="2535" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PL01" sheetId="5" r:id="rId1"/>
@@ -2455,9 +2455,6 @@
     <t>Như PL01 của báo cáo tuần, nguồn dữ liệu B02.00 từ tháng 1 đến tháng BC</t>
   </si>
   <si>
-    <t>Nguồn dữ liệu B01-10  để lấy số thực chi (T_BHTT)</t>
-  </si>
-  <si>
     <t>Số thông báo số dự kiến chi  vớt vào từ file excel, lưu riêng 1 bảng cho từng đợt báo cáo.</t>
   </si>
   <si>
@@ -2496,6 +2493,9 @@
   </si>
   <si>
     <t>Cách lập giống như Phụ lục 03 báo cáo tuần, nguồn dữ liệu lấy từ B02-10-2024 của tháng báo cáo</t>
+  </si>
+  <si>
+    <t>Nguồn dữ liệu B02-10  để lấy số thực chi (T_BHTT)</t>
   </si>
 </sst>
 </file>
@@ -12594,7 +12594,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1452" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -12915,8 +12915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13210,17 +13210,17 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1519" t="s">
-        <v>808</v>
+        <v>821</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1519" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -13273,7 +13273,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="1532" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
@@ -14048,7 +14048,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C1" s="1523" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="42.75" x14ac:dyDescent="0.25">
@@ -14817,7 +14817,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="1523" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
@@ -18939,7 +18939,7 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
   </sheetData>
@@ -18968,7 +18968,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="1523" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
@@ -23090,7 +23090,7 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B183" s="1535" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
   </sheetData>
@@ -23116,7 +23116,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="1523" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
@@ -23730,7 +23730,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
   </sheetData>
@@ -23755,7 +23755,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="1523" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
@@ -23772,7 +23772,7 @@
         <v>88</v>
       </c>
       <c r="E3" s="1534" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>90</v>
@@ -24325,7 +24325,7 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="1533" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>